<commit_message>
added tasks and 2 labs
</commit_message>
<xml_diff>
--- a/Задачи на 1 семестр/Задачи.xlsx
+++ b/Задачи на 1 семестр/Задачи.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manan\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manan\Downloads\Задачи на 1 семестр\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D4BAB9F-59A6-4D3D-9718-B789EBE7DFFA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30293BA5-A1D9-479F-BDE9-3F7EEEAAE4A2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{08E66B02-90A5-4DBE-B310-89731172CFD8}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="114">
   <si>
     <t>Найти уравнение прямой, проходящей через две заданные пользователем точки координатной плоскости. Уравнение любой прямой имеет вид y = kx + b. Если известны две пары (x; y), то получают систему уравнений относительно коэффициентов k и b:</t>
   </si>
@@ -425,6 +425,35 @@
   </si>
   <si>
     <t xml:space="preserve">Пользователь вводит числа a и b. Сгенерировать случайные числа в интервале [a;b] и заполнить ими двумерный массив размером 10 на 10. В массиве необходимо найти максимальный и минимальный элемент. Заменить числа на главной диагонали на максимальный элемент, а числа на побочной - на минимальный. На место пересечения - сумму максимального и минимального. Вывести на экран. </t>
+  </si>
+  <si>
+    <t>Пользователь вводит через запятую целые числа, которыми будет заполнен массив.  Напишите функцию, которая принимает массив с разными числами, а возвращает максимальное произведение двух чисел из этого массива. Вывести результат.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Входные данные:
+[1, 3, 2, 2, 3, 0]
+Выходные данные:
+9
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Пользователь вводит строку. Напишите функцию, которая принимает строку, а возвращает ее перевернутый вариант (слова в обратном порядке). Напечатать полученную строку на экране. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Входные данные:
+“general purpose programming language” 
+Выходные данные:
+“language programming purpose general”
+</t>
+  </si>
+  <si>
+    <t>На вход подается число N. Вывести на экран треугольник из символов ’*’ из N линий.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Пользователь вводит числа, которыми будет заполнен массив. Реализовать функцию сортировки массива. Вывести на экран отсортированный массив. </t>
+  </si>
+  <si>
+    <t>На вход подается одномерный массив целых чисел. Необходимо отсортировать массив (можно методом пузырька) и вывести его на экран. В отсортированном массиве найти медиану (отметка, делящая ранжированные данные, либо число по середине ранжированного списка либо среднее арифметическое из двух по середине), моду (наиболее часто встречающееся значение в данных), среднее, максимум, минимум, размах (разность между наибольшим и наименьшим).</t>
   </si>
 </sst>
 </file>
@@ -520,7 +549,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -532,6 +561,12 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -850,8 +885,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CB57B17-6A15-45A5-8FFE-C15181C6CFB2}">
   <dimension ref="A1:D60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1284,33 +1319,47 @@
       <c r="C33" s="4"/>
       <c r="D33" s="4"/>
     </row>
-    <row r="34" spans="1:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
-      <c r="B34" s="4"/>
-      <c r="C34" s="4"/>
+      <c r="B34" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>108</v>
+      </c>
       <c r="D34" s="4"/>
     </row>
-    <row r="35" spans="1:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
-      <c r="B35" s="4"/>
-      <c r="C35" s="4"/>
+      <c r="B35" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>110</v>
+      </c>
       <c r="D35" s="4"/>
     </row>
     <row r="36" spans="1:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
-      <c r="B36" s="4"/>
+      <c r="B36" s="6" t="s">
+        <v>111</v>
+      </c>
       <c r="C36" s="4"/>
       <c r="D36" s="4"/>
     </row>
     <row r="37" spans="1:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
-      <c r="B37" s="4"/>
+      <c r="B37" s="4" t="s">
+        <v>112</v>
+      </c>
       <c r="C37" s="4"/>
       <c r="D37" s="4"/>
     </row>
-    <row r="38" spans="1:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" ht="98.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
-      <c r="B38" s="4"/>
+      <c r="B38" s="4" t="s">
+        <v>113</v>
+      </c>
       <c r="C38" s="4"/>
       <c r="D38" s="4"/>
     </row>

</xml_diff>